<commit_message>
new o blindness heuristics
</commit_message>
<xml_diff>
--- a/stats/heuristics_fitted_combinations_with_oBlind_23052018.xlsx
+++ b/stats/heuristics_fitted_combinations_with_oBlind_23052018.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="345" windowWidth="19875" windowHeight="5670"/>
+    <workbookView xWindow="0" yWindow="345" windowWidth="19875" windowHeight="5670" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="heuristics_fitted_combinations_" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
     <sheet name="fewer" sheetId="2" r:id="rId3"/>
+    <sheet name="new30052018" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">fewer!$A$1:$J$347</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="23" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -5585,7 +5586,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -5925,7 +5926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S347"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
@@ -38622,4 +38623,16 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>